<commit_message>
Access numeric cell type from excel
</commit_message>
<xml_diff>
--- a/Demo Data.xlsx
+++ b/Demo Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwokl\Udemy\Rest API Testing (Automation) from Scratch-Rest Assured Java\ExcelDrivenTestFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0B9F4C-E2FC-4283-A503-5CB88CE92F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593FAE45-7DC6-4FCE-BB26-04A6116F89A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{BA87C6E2-647F-4207-ACC4-7AE158428664}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Testcases</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>oiu</t>
-  </si>
-  <si>
-    <t>ghjkg</t>
   </si>
   <si>
     <t>cvbn</t>
@@ -458,7 +455,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,11 +512,11 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -527,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>